<commit_message>
All variables extracted except VIS
</commit_message>
<xml_diff>
--- a/analysis/eICU_MIMIC_MatchUp.xlsx
+++ b/analysis/eICU_MIMIC_MatchUp.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sreekar\Documents\HST.953\953-2019-team_i\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2CC3AA-AA46-4B0E-97D4-D3D7AF8763E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E445937A-26A7-424F-9407-024CDD17E91D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BEE65E1E-AC63-469E-B669-A34AED340DDB}"/>
+    <workbookView xWindow="6690" yWindow="225" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{BEE65E1E-AC63-469E-B669-A34AED340DDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="242">
   <si>
     <t>subject_id</t>
   </si>
@@ -640,16 +638,155 @@
   </si>
   <si>
     <t>only 18k</t>
+  </si>
+  <si>
+    <t>working on it</t>
+  </si>
+  <si>
+    <t>cardiac_arrest_and_ventricular_fibrillation + shock_index + vent + sp_o2_mean + bun_max + charlson_score + any_pressor</t>
+  </si>
+  <si>
+    <t>wide_ccu_dx,</t>
+  </si>
+  <si>
+    <t>ccu_vitals,</t>
+  </si>
+  <si>
+    <t>ccu_labs,</t>
+  </si>
+  <si>
+    <t>ccu_patients_id_los,</t>
+  </si>
+  <si>
+    <t>ccu_demographics_dob_gender_death,</t>
+  </si>
+  <si>
+    <t>ccu_uo_24h,</t>
+  </si>
+  <si>
+    <t>ccu_RRT24h,</t>
+  </si>
+  <si>
+    <t>ccu_vent,</t>
+  </si>
+  <si>
+    <t>wide_procedures_24,</t>
+  </si>
+  <si>
+    <t>wide_pressors,</t>
+  </si>
+  <si>
+    <t>wide_pressors_firsthour,</t>
+  </si>
+  <si>
+    <t>ccu_gcs,</t>
+  </si>
+  <si>
+    <t>ccu_sofa,</t>
+  </si>
+  <si>
+    <t>ccu_oasis,</t>
+  </si>
+  <si>
+    <t>wide_cabg_pci,</t>
+  </si>
+  <si>
+    <t>ccu_mortality,</t>
+  </si>
+  <si>
+    <t>charlson9,</t>
+  </si>
+  <si>
+    <t>vis_24h,</t>
+  </si>
+  <si>
+    <t>vis_first_hour,</t>
+  </si>
+  <si>
+    <t>nee_24h,</t>
+  </si>
+  <si>
+    <t>nee_first_hour,</t>
+  </si>
+  <si>
+    <t>ccu_race+F17:X17</t>
+  </si>
+  <si>
+    <t>Yes, only 20k patients</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>may  not be accurate</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>dialysis, correct?</t>
+  </si>
+  <si>
+    <t>actually gets all dialysis, not marked in eicu</t>
+  </si>
+  <si>
+    <t>seems like a much higher proportion of mimic patients actually got this</t>
+  </si>
+  <si>
+    <t>https://eicu-crd.mit.edu/eicutables/respiratorycare/</t>
+  </si>
+  <si>
+    <t>impella, iabp, ecmo</t>
+  </si>
+  <si>
+    <t>can do by searching or icd9</t>
+  </si>
+  <si>
+    <t>not really</t>
+  </si>
+  <si>
+    <t>how did you define first hour, etc?</t>
+  </si>
+  <si>
+    <t>lots of different gcs values, I just took mininum</t>
+  </si>
+  <si>
+    <t>races are just in a different format</t>
+  </si>
+  <si>
+    <t>tech yes</t>
+  </si>
+  <si>
+    <t>not sure if the correct moratlity was ued</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -693,15 +830,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,19 +857,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="MyData"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1029,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E540EFD2-E081-49B9-ADED-5FC69D3054DB}">
   <dimension ref="B1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B53" sqref="B52:B53"/>
+    <sheetView topLeftCell="A31" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,6 +1947,9 @@
       <c r="B93" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="C93" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="D93" s="1" t="s">
         <v>104</v>
       </c>
@@ -2017,4 +2149,226 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37A2ADF-A371-4019-928A-926604A35FC4}">
+  <dimension ref="B8:G36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="51.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G22" r:id="rId1" xr:uid="{48290A45-9B61-4AA7-8BD7-F79BE3608227}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Joined data file for eICU
</commit_message>
<xml_diff>
--- a/analysis/eICU_MIMIC_MatchUp.xlsx
+++ b/analysis/eICU_MIMIC_MatchUp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sreekar\Documents\HST.953\953-2019-team_i\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EE984E-0662-49D8-9C6F-7F82F646D367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810559B7-BBE3-48D0-BFA9-CA0B6A437389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BEE65E1E-AC63-469E-B669-A34AED340DDB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="257">
   <si>
     <t>subject_id</t>
   </si>
@@ -794,6 +794,15 @@
   </si>
   <si>
     <t>updated so that only 0 to 24 and then 0 to 1, correct? Chartoffset</t>
+  </si>
+  <si>
+    <t>length(grep("367.1", clean_icd9$ICD9_code))</t>
+  </si>
+  <si>
+    <t>I tried searching by ICD-9, but it doesn't return any results. Maybe it's just diagnosis codes?</t>
+  </si>
+  <si>
+    <t>added pH, not sure why troponin so low</t>
   </si>
 </sst>
 </file>
@@ -889,7 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -912,6 +921,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2228,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37A2ADF-A371-4019-928A-926604A35FC4}">
   <dimension ref="B8:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,7 +2356,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>212</v>
       </c>
@@ -2356,6 +2368,12 @@
       </c>
       <c r="E23" s="3" t="s">
         <v>233</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -2390,7 +2408,7 @@
       <c r="D26" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="10" t="s">
         <v>246</v>
       </c>
     </row>
@@ -2474,6 +2492,9 @@
       </c>
       <c r="C41" s="3" t="s">
         <v>245</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added updated .csv file for eICU
</commit_message>
<xml_diff>
--- a/analysis/eICU_MIMIC_MatchUp.xlsx
+++ b/analysis/eICU_MIMIC_MatchUp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sreekar\Documents\HST.953\953-2019-team_i\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810559B7-BBE3-48D0-BFA9-CA0B6A437389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5D32C2-A762-4529-82F3-06CDECD55783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BEE65E1E-AC63-469E-B669-A34AED340DDB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="260">
   <si>
     <t>subject_id</t>
   </si>
@@ -760,9 +760,6 @@
     <t>maybe due to patient population</t>
   </si>
   <si>
-    <t>just use icd9 code</t>
-  </si>
-  <si>
     <t>changet his to treatment table and stratify first 24 hours</t>
   </si>
   <si>
@@ -803,6 +800,18 @@
   </si>
   <si>
     <t>added pH, not sure why troponin so low</t>
+  </si>
+  <si>
+    <t>CHANGE table to RRTTreatment</t>
+  </si>
+  <si>
+    <t>add that back iabp</t>
+  </si>
+  <si>
+    <t>Ask about it, icd9 code is not working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">look into </t>
   </si>
 </sst>
 </file>
@@ -898,7 +907,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -924,6 +933,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2240,8 +2252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37A2ADF-A371-4019-928A-926604A35FC4}">
   <dimension ref="B8:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,7 +2327,7 @@
         <v>239</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="105" x14ac:dyDescent="0.25">
@@ -2332,10 +2344,13 @@
         <v>240</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -2352,7 +2367,7 @@
         <v>241</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J22" s="7"/>
     </row>
@@ -2370,10 +2385,13 @@
         <v>233</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -2384,7 +2402,7 @@
         <v>227</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -2409,7 +2427,7 @@
         <v>236</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -2417,7 +2435,7 @@
         <v>216</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -2425,7 +2443,7 @@
         <v>217</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -2433,7 +2451,10 @@
         <v>218</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>242</v>
+        <v>258</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -2444,7 +2465,7 @@
         <v>238</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2488,13 +2509,13 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>245</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>